<commit_message>
woring on patient editor
</commit_message>
<xml_diff>
--- a/MVCSchooldbDemo/Docs/EditorDesign.xlsx
+++ b/MVCSchooldbDemo/Docs/EditorDesign.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -563,29 +564,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="23.75" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.08203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.25" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.25" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2"/>
     </row>
-    <row r="2" spans="1:9" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -606,7 +607,7 @@
       </c>
       <c r="I2" s="2"/>
     </row>
-    <row r="3" spans="1:9" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
@@ -624,11 +625,11 @@
       </c>
       <c r="I3" s="3"/>
     </row>
-    <row r="4" spans="1:9" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:9" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
       <c r="D4" t="s">
         <v>10</v>
       </c>
@@ -638,12 +639,12 @@
       </c>
       <c r="G4" s="3"/>
     </row>
-    <row r="5" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -657,7 +658,7 @@
       </c>
       <c r="F6" s="2"/>
     </row>
-    <row r="7" spans="1:9" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -671,7 +672,7 @@
       </c>
       <c r="F7" s="2"/>
     </row>
-    <row r="8" spans="1:9" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -680,18 +681,18 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>22</v>
       </c>
       <c r="B9" s="2"/>
     </row>
-    <row r="10" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -709,7 +710,7 @@
       </c>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:9" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -727,7 +728,7 @@
       </c>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:9" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>32</v>
       </c>
@@ -745,7 +746,7 @@
       </c>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:9" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>36</v>
       </c>
@@ -757,7 +758,7 @@
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
     </row>
-    <row r="15" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>37</v>
       </c>
@@ -769,7 +770,7 @@
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
     </row>
-    <row r="16" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>38</v>
       </c>
@@ -787,7 +788,7 @@
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>
     </row>
-    <row r="17" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>42</v>
       </c>
@@ -810,4 +811,19 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>